<commit_message>
Aggiunge Stats di base
</commit_message>
<xml_diff>
--- a/Incremental/Resources/Virtus e Stats Base.xlsx
+++ b/Incremental/Resources/Virtus e Stats Base.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21735" windowHeight="8025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20955" windowHeight="7035"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Volontà</t>
   </si>
   <si>
-    <t>Exedia</t>
-  </si>
-  <si>
     <t>CORAGGIO</t>
   </si>
   <si>
@@ -181,13 +178,16 @@
     <t>VOLONTA'</t>
   </si>
   <si>
-    <t>+ Danno Exedia</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>+ PA</t>
+  </si>
+  <si>
+    <t>Puro</t>
+  </si>
+  <si>
+    <t>+ Danno Puro</t>
   </si>
 </sst>
 </file>
@@ -378,9 +378,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -401,6 +398,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -684,7 +684,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,19 +702,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="E1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="14"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -732,17 +732,17 @@
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="30" t="s">
-        <v>38</v>
+      <c r="J2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -756,17 +756,17 @@
       <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>29</v>
+      <c r="J3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -787,24 +787,24 @@
       <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="19" t="s">
+      <c r="J4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="18" t="s">
         <v>35</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -818,17 +818,17 @@
       <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>31</v>
+      <c r="J5" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -861,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -872,17 +872,17 @@
       <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="30" t="s">
+      <c r="J7" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="30" t="s">
-        <v>45</v>
+      <c r="M7" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -903,17 +903,17 @@
       <c r="G8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>47</v>
+      <c r="J8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -932,19 +932,19 @@
         <v>2</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -953,17 +953,17 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L10" s="16" t="s">
+      <c r="J10" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="25" t="s">
         <v>55</v>
-      </c>
-      <c r="M10" s="26" t="s">
-        <v>53</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -983,28 +983,28 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>52</v>
+      <c r="J12" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>35</v>
+      <c r="J13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1012,30 +1012,30 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="F14" s="5"/>
-      <c r="J14" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="K14" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="L14" s="32" t="s">
-        <v>55</v>
+      <c r="J14" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="31" t="s">
+        <v>53</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J15" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="27" t="s">
-        <v>43</v>
+      <c r="J15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>

</xml_diff>

<commit_message>
PRIMA DI MODIFICARE TUTTO IL REDIRECT
</commit_message>
<xml_diff>
--- a/Incremental/Resources/Virtus e Stats Base.xlsx
+++ b/Incremental/Resources/Virtus e Stats Base.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FCEDF420-F680-44B3-84C8-93D4B747A937}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21705" windowHeight="8160" tabRatio="285"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21765" windowHeight="15090" tabRatio="285" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PANORAMICA" sheetId="1" r:id="rId1"/>
     <sheet name="VIRTUS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M19"/>
+  <oleSize ref="A1:U24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -212,7 +213,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -636,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,11 +1019,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>